<commit_message>
change to title displayed
</commit_message>
<xml_diff>
--- a/Algo Results.xlsx
+++ b/Algo Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Desktop/horse_race_predictor/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CCD743-BC62-B44F-9C48-84678E8C925D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5C7685-CC43-B146-BA1F-FED0024E8B2D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="18000" xr2:uid="{413A8F49-1818-2247-93E6-602FB06B00A9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{413A8F49-1818-2247-93E6-602FB06B00A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -990,7 +990,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{249ABB75-DFE5-D549-98A5-A9C17DF4CEB1}">
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>

</xml_diff>